<commit_message>
Update BOM anf cable's file
</commit_message>
<xml_diff>
--- a/Docs/AT-ETX-2i10G.CBL04.xlsx
+++ b/Docs/AT-ETX-2i10G.CBL04.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDocuments\ate\AutoTesters\TCL\ETX-2i-10G\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5D9338-795E-4C42-8A01-CD707382B05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F06E057-92C0-41D4-941F-B875B03F3BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2610" yWindow="1455" windowWidth="20895" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5205" yWindow="480" windowWidth="21945" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -327,7 +327,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,11 +1054,11 @@
         <v>10</v>
       </c>
       <c r="C39" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39" s="3">
         <f>$C$35*C39</f>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>